<commit_message>
Added more tests and support for the pump system.
</commit_message>
<xml_diff>
--- a/test_protocol.xlsx
+++ b/test_protocol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="11" documentId="8_{788ADA4C-2D56-7345-A8A8-07B0308A7C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1989E473-69B8-2145-B1FD-2852A7A8C65E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Established connection to pumps
</commit_message>
<xml_diff>
--- a/test_protocol.xlsx
+++ b/test_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{788ADA4C-2D56-7345-A8A8-07B0308A7C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1989E473-69B8-2145-B1FD-2852A7A8C65E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F469E5-886C-422E-993B-8CEE961C6CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Pump</t>
   </si>
@@ -52,18 +52,6 @@
   </si>
   <si>
     <t>F.0.1.22_1</t>
-  </si>
-  <si>
-    <t>F.0.1.22_2</t>
-  </si>
-  <si>
-    <t>F.0.1.22_3</t>
-  </si>
-  <si>
-    <t>F.0.1.22_4</t>
-  </si>
-  <si>
-    <t>F.0.1.21_1</t>
   </si>
 </sst>
 </file>
@@ -541,16 +529,16 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="29" width="9.6640625" style="7" customWidth="1"/>
+    <col min="1" max="29" width="9.625" style="7" customWidth="1"/>
     <col min="30" max="32" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -600,7 +588,7 @@
       <c r="AE1"/>
       <c r="AF1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -650,31 +638,15 @@
       <c r="AE2"/>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="11">
-        <v>1440</v>
-      </c>
-      <c r="E3" s="12">
-        <v>5.6</v>
-      </c>
-      <c r="F3" s="12">
-        <v>6.8</v>
-      </c>
-      <c r="G3" s="13">
-        <v>5</v>
-      </c>
-      <c r="H3" s="13">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
@@ -700,31 +672,15 @@
       <c r="AE3"/>
       <c r="AF3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11">
-        <v>1440</v>
-      </c>
-      <c r="E4" s="12">
-        <v>5.6</v>
-      </c>
-      <c r="F4" s="12">
-        <v>6.8</v>
-      </c>
-      <c r="G4" s="13">
-        <v>5</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
@@ -750,31 +706,15 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11">
-        <v>1440</v>
-      </c>
-      <c r="E5" s="12">
-        <v>5.6</v>
-      </c>
-      <c r="F5" s="12">
-        <v>6.8</v>
-      </c>
-      <c r="G5" s="13">
-        <v>5</v>
-      </c>
-      <c r="H5" s="13">
-        <v>1</v>
-      </c>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -800,31 +740,15 @@
       <c r="AE5"/>
       <c r="AF5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="11">
-        <v>1440</v>
-      </c>
-      <c r="E6" s="12">
-        <v>5.6</v>
-      </c>
-      <c r="F6" s="12">
-        <v>6.8</v>
-      </c>
-      <c r="G6" s="13">
-        <v>5</v>
-      </c>
-      <c r="H6" s="13">
-        <v>1</v>
-      </c>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
@@ -850,7 +774,7 @@
       <c r="AE6"/>
       <c r="AF6"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -876,7 +800,7 @@
       <c r="AE7"/>
       <c r="AF7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -910,7 +834,7 @@
       <c r="AE8"/>
       <c r="AF8"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
@@ -927,7 +851,7 @@
       <c r="AE9"/>
       <c r="AF9"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
@@ -944,7 +868,7 @@
       <c r="AE10"/>
       <c r="AF10"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
@@ -961,7 +885,7 @@
       <c r="AE11"/>
       <c r="AF11"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>

</xml_diff>

<commit_message>
Added tests for pump initial setup
</commit_message>
<xml_diff>
--- a/test_protocol.xlsx
+++ b/test_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F469E5-886C-422E-993B-8CEE961C6CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{788ADA4C-2D56-7345-A8A8-07B0308A7C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4713AB-06A8-A54E-BDEC-618C65C14296}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Pump</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>F.0.1.22_1</t>
+  </si>
+  <si>
+    <t>F.0.1.22_2</t>
+  </si>
+  <si>
+    <t>F.0.1.22_3</t>
+  </si>
+  <si>
+    <t>F.0.1.22_4</t>
+  </si>
+  <si>
+    <t>F.0.1.21_1</t>
   </si>
 </sst>
 </file>
@@ -529,16 +541,16 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="29" width="9.625" style="7" customWidth="1"/>
+    <col min="1" max="29" width="9.6640625" style="7" customWidth="1"/>
     <col min="30" max="32" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -588,7 +600,7 @@
       <c r="AE1"/>
       <c r="AF1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -638,15 +650,31 @@
       <c r="AE2"/>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E3" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F3" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G3" s="13">
+        <v>10</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1</v>
+      </c>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
@@ -672,15 +700,31 @@
       <c r="AE3"/>
       <c r="AF3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E4" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F4" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G4" s="13">
+        <v>15</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1</v>
+      </c>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
@@ -706,15 +750,31 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E5" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F5" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G5" s="13">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -740,15 +800,31 @@
       <c r="AE5"/>
       <c r="AF5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E6" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F6" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G6" s="13">
+        <v>5</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
@@ -774,7 +850,7 @@
       <c r="AE6"/>
       <c r="AF6"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -800,7 +876,7 @@
       <c r="AE7"/>
       <c r="AF7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -834,7 +910,7 @@
       <c r="AE8"/>
       <c r="AF8"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
@@ -851,7 +927,7 @@
       <c r="AE9"/>
       <c r="AF9"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
@@ -868,7 +944,7 @@
       <c r="AE10"/>
       <c r="AF10"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
@@ -885,7 +961,7 @@
       <c r="AE11"/>
       <c r="AF11"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>

</xml_diff>

<commit_message>
Added integration test for whole system
</commit_message>
<xml_diff>
--- a/test_protocol.xlsx
+++ b/test_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{788ADA4C-2D56-7345-A8A8-07B0308A7C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4713AB-06A8-A54E-BDEC-618C65C14296}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{788ADA4C-2D56-7345-A8A8-07B0308A7C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC82A232-3B0A-A24A-9942-CC8E46E9B1AF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,7 +623,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -673,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -723,7 +723,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -773,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>

</xml_diff>

<commit_message>
Fixed an error when establishing connection with the pumps
</commit_message>
<xml_diff>
--- a/test_protocol.xlsx
+++ b/test_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{788ADA4C-2D56-7345-A8A8-07B0308A7C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC82A232-3B0A-A24A-9942-CC8E46E9B1AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AFFFA1-1543-48A8-9180-C189686E15FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,16 +541,16 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="29" width="9.6640625" style="7" customWidth="1"/>
+    <col min="1" max="29" width="9.625" style="7" customWidth="1"/>
     <col min="30" max="32" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -600,7 +600,7 @@
       <c r="AE1"/>
       <c r="AF1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -620,7 +620,7 @@
         <v>6.8</v>
       </c>
       <c r="G2" s="13">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="H2" s="13">
         <v>5</v>
@@ -650,7 +650,7 @@
       <c r="AE2"/>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="AE3"/>
       <c r="AF3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -750,7 +750,7 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="AE5"/>
       <c r="AF5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -850,7 +850,7 @@
       <c r="AE6"/>
       <c r="AF6"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -876,7 +876,7 @@
       <c r="AE7"/>
       <c r="AF7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -910,7 +910,7 @@
       <c r="AE8"/>
       <c r="AF8"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
@@ -927,7 +927,7 @@
       <c r="AE9"/>
       <c r="AF9"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
@@ -944,7 +944,7 @@
       <c r="AE10"/>
       <c r="AF10"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
@@ -961,7 +961,7 @@
       <c r="AE11"/>
       <c r="AF11"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>

</xml_diff>